<commit_message>
after full database double-check
</commit_message>
<xml_diff>
--- a/data/ten_journals/per_observer/ten_journals_fulltext_screening_and_data_extraction_AST.xlsx
+++ b/data/ten_journals/per_observer/ten_journals_fulltext_screening_and_data_extraction_AST.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1945" uniqueCount="692">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1991" uniqueCount="693">
   <si>
     <t>studyID</t>
   </si>
@@ -1776,15 +1776,9 @@
     <t>both</t>
   </si>
   <si>
-    <t>Repeatabilities were estimated as the intraclass coefficient at the individual level from [a model with] individuals' identities and cohort as random effects. [...] interindividual variation in exploration remained consistent across time and contexts. Thus, our test identified the well-known fasteslow exploration continuum, with some individuals consistently exploring both space and objects more than others. [...] We also need to assess how repeatable the measures are across time, which is a prerequisite for classifying the behaviour as a personality trait.</t>
-  </si>
-  <si>
     <t>among</t>
   </si>
   <si>
-    <t>among?</t>
-  </si>
-  <si>
     <t>We found considerable variability in foraging activity and aggressive behavior among fish individuals (Figure 4) [...] The results showed strong individual variation in aggression toward newts, with a high repeatability score</t>
   </si>
   <si>
@@ -1809,9 +1803,6 @@
     <t>First, we assessed the level of individual repeatability of each response trait and the correlations among them [...] The significance of the repeatability (i.e. variance explained by between individual differences) was tested using a likelihood ratio test by comparing the model with individual as random effect to an alternative model without this random effect. [...] While the repeatability of traits involved can inform on the stability of impacts of intraspecific trait variability on ecosystem functioning, we suggest that functional syndromes may result from correlations among traits arising from both intra- and interindividual covariations of traits [54,55] and might therefore not require the repeatability of all traits involved in the syndrome</t>
   </si>
   <si>
-    <t>The interpretation of repeatability assigned as within, despite that repeatability is defined as: repeatability (i.e. variance explained by between individual differences), in the methods.</t>
-  </si>
-  <si>
     <t>Individuals displayed consistent behavioural and physiological states, which may explain the temporal consistency of effect traits because of their interconnections. Importantly, we confirmed that effect traits could be repeatable over a relatively long period of crayfish lifetime (here 71 days, e.g. [61]), indicating that the effects of phenotypic variability on ecosystem functioning could be stable throughout individual life. [...] Quantifying the temporal consistency and environmental dependency of the functional syndrome should provide an integrative understanding of the ecosystem response to phenotypic variability.</t>
   </si>
   <si>
@@ -1839,21 +1830,12 @@
     <t>Repeatability measured as a regression between individual behaviour measured at two different times, instead of using variance partitioning. Repeatability nonetheless interpreted as individual consistency: Consistency of behavior: Consistency is represented by a significant effect of the first time a behavior was measured on the second measure of the same behavior in linear models (Table 2). Male domestic fowl showed significant among-individual consistency in aggression, activity, boldness, and crowing (Figure 2, Table 2). Vigilance and exploration showed positive but nonsignificant correlations across time and treatment (Figure 2, Table 2).</t>
   </si>
   <si>
-    <t>yes?</t>
-  </si>
-  <si>
     <t>Repeatability estimates did not differ between treatment groups and the whole sample. Therefore, in the case of activity, we could not support either of our hypotheses regarding short-term environmental effects on behavioural consistency. [...] Repeatability of shelter use was negligible, except in the high food × vitamin D3 group where it was moderately repeatable and in the pooled sample where it was weak (see Bell et al. 2009) (Table 1). This suggests that the emergence of ‘shelter use personality’ is environment-dependent as between-individual variation increased under the best conditions offered by our treatments. [...] For instance, it is plausible that individuals under favourable environmental conditions can allow ‘extreme’ behavioural strategies, which increases the between-individual component of variance. This assumption is supported by a recent experimental study (Lichtenstein et al. 2016). Environmental effects on yearly variation in presence/ absence/strength of behavioural consistency have been also supported in different wild bird populations (Dingemanse et al. 2004; Garamszegi et al. 2015). There was no indication of higher repeatability in the pooled sample compared to the treatment groups; therefore, we reject the hypothesis about lowered environmental variation weakening shelter use personality.</t>
   </si>
   <si>
     <t>We tested whether changing labile components of individual state affected (i) behavioural consistency (the degree of between-individual difference) and (ii) behavioural type (mean behaviour) [...] We conclude that short-term changes in individual state affect both behavioural consistency and behavioural type of reproductive male I. cyreni. Unfavourable conditions resulted in decreased behavioural consistency, while high-state individuals became less active in general. [...] Further, social and environmental conditions during early life seem to have a fundamental role in the emergence of behavioural consistency during early stages of ontogeny [...] However, effects of short-term differences in internal state or environmental conditions on behavioural consistency during late ontogeny are not obvious [...] Whether state-dependence of behavioural consistency exists during adulthood and the strength of behavioural consistency could change during short time periods [...] In our study, by manipulating the quantity and quality of diet for more than 2 weeks during the short and highly synchronized mating season of I. cyreni (Martín and Salvador 1992), we could not affect the consistency of activity, but the presence/absence of animal personality in shelter use and risk taking was environment-dependent. [...] We consider risk-taking personality being present in three out of the four treatment groups and also in the pooled sample. Such pattern could be explained similarly to the pattern seen in shelter use: individuals under unfavourable environmental conditions tend to shift their behaviour towards a general strategy, resulting in decreased between-individual variation (Lichtenstein et al. 2016). [...] We suggest that behavioural consistency is—on some level—affected by short-term ecological conditions in the studied population of adult male I. cyreni during the mating season. Hence, environmental conditions are likely responsible not only for the longterm development, but also for the short-term maintenance of individual behavioural variation.</t>
   </si>
   <si>
-    <t>both?</t>
-  </si>
-  <si>
-    <t>We tested whether changing labile components of individual state affected (i) behavioural consistency (the degree of between-individual difference) and (ii) behavioural type (mean behaviour) [...] We suggest that behavioural consistency is—on some level—affected by short-term ecological conditions in the studied population of adult male I. cyreni during the mating season. Hence, environmental conditions are likely responsible not only for the longterm development, but also for the short-term maintenance of individual behavioural variation. [...] As our behavioural assays covered an 8-day interval, we cannot claim that we report ‘true’ personalities that are consistent over long periods. [...] By showing that differences in environmental conditions cannot only shift the mean behaviour in animal groups during a short timeframe, but it might affect the level of between-individual variation too, we demonstrated the liability of behavioural consistency.</t>
-  </si>
-  <si>
     <t>Repeatability was calculated to measure consistent participation by individuals using the ‘rptR’ package (Schielzeth and Nakagawa 2011) in R (R Core Team 2009). [...] Individuals exhibited consistent differences in prey capture in all colonies, as evidenced by significant variation at the random intercept between individuals (Fig. 2, Table 1). In contrast to prey capture, spiders did not exhibit consistency in web maintenance (Fig. 3, Table 1). [...] Here, we show that behavioural consistency seen in prey capture over the short term also persists over a considerable part of the adulthood of spiders. The model for prey capture indicated behavioural consistency, while repeatability scores for individual participation were low.</t>
   </si>
   <si>
@@ -1872,9 +1854,6 @@
     <t>Significant variation between individuals (random intercepts) allowed estimation of repeatability. Startle responses were very consistent with each other when measured twice in a novel and twice in a non-novel environment (Figure 1). Accordingly, repeatability across the four replicates, corrected by claw size, was high and different from zero in all three sites (Table 2). [...] We found no significant differences in consistency or plasticity among habitats. One potential explanation is that the cost of developing cognitive structures necessary for plasticity (Dall et al., 2004; Hazlett, 1995) may be too high in hermit crabs generally, so consistency is favored in all habitats (Bell, 2007; Briffa et al., 2008). This is supported by the high repeatability found across habitats (substantially higher than the average of ~0.4 reported in field studies across taxa; Bell et al., 2009). The lack of differences in consistency could also be explained by the limited capacity C. compressus has for local adaption, as mentioned above. However, it is possible that the behavioral assays were conducted in too short a time frame to accurately detect plasticity; thus, these results should be interpreted with caution.</t>
   </si>
   <si>
-    <t>We found that individual differences in behavior were overall repeatable over ontogeny (i.e., personality was manifested). [...] Since we were interested in testing whether personality was manifested in genetically similar mosquitofish, we used the resulting among-individual and within-individual variance estimates from the LMMs described above to estimate the overall repeatability of each behavioral trait over fish ontogeny (Nakagawa and Schielzeth 2010; Dingemanse and Dochtermann 2013). Repeatability represents the proportion of behavioral variation attributable to consistent differences among individuals (Dingemanse and Dochtermann 2013). [...] To test whether the within- and the among-individual variance for a given behavioral trait increased or decreased over the ontogeny, we estimated both within- and amongindividual variances for each behavior at each stage by using a MCMC sampling method [...] Across the entire experimental campaign, we detected personality differences among fish for each of the four behavioral traits measured, suggesting that individual differences in behavior were overall repeatable over the ontogeny of mosquitofish (Table 1). Nevertheless, the overall repeatability of fish behavior across the ontogeny was low (Table 1). [...] Furthermore, we observed a significant decline in the within-individual behavioral variance over ontogeny that was consistent to all behavioral traits for which personality was detected (Table 3; Fig. 4), whereas the among-individual variance did not vary with fish age for any trait (Table 3; Fig. 4).</t>
-  </si>
-  <si>
     <t>Consistency measured via correlations. Repeatability not mentioned.</t>
   </si>
   <si>
@@ -1914,12 +1893,6 @@
     <t>Repeatability was tested using intraclass correlation in the psych package, using ICC1 (standard repeatability sensu Lessells &amp; Boag (1987)) and ICC3 (standardized for overall change in trait mean between time points, time treated as a fixed factor). [...] Results All personality traits (exploration, boldness, activity) were significantly repeatable (Table 1a). Coloration and morphological traits were also highly repeatable across measurements, with a stronger repeatability when the ICC3 was used (i.e. accounting for population- level change in trait expression between trials 1 and 2) (Table 1b). [...] The resulting temporal change of individual AMB in the course of 5 wk and relative stability of personality traits suggest higher flexibility of AMB. It seems that personality traits are relatively fixed in a short timescale compared with more flexible AMB. It is notable because a dramatic change in the social environment was predicted to at least slightly influence the expression of personality traits assuming that different traits are favoured in different environments. As a result, social environments in this experiment only influenced AMB while personality traits remained unchanged.</t>
   </si>
   <si>
-    <t>First, we ran univariate models to calculate repeatability of behavioural traits. To do so, we decomposed the variance into within-individual (VW) and among-individual (VA) components, and repeatability (r) was calculated as VA VAþVW . [...] Differences in personality may reflect genetic differences, phenotypic plasticity or flexibility (changes in behaviour resulting from environmental change), or all of these [...] Behavioural traits measured in the open field were repeatable (Table 1) and thus we can conclude that individual Siberian hamsters have different personalities, although these differences did not correlate with differences in winter phenotype.</t>
-  </si>
-  <si>
-    <t>there were consistent individual differences in cortisol release rate over time, with some individuals consistently releasingmore cortisol than others across the two sampling periods (repeata-bility of sample average, R = 0.6159 [0.2252, 0.9218], n = 10, Fig. 2b). [...] There were consistent individual differences in boldness across the four measurements (R = 0.4980 [0.0817, 0.8244], n = 10, Fig. 3a). [...] We observed strong inter-individual variation among wild-caught individual sticklebacks from a natural population [...] For example, some sticklebacks were consistently more bold than others toward a model predator. [...] Additionally, we also observed that some individual sticklebacks were consistently morestress reactive than others.</t>
-  </si>
-  <si>
     <t>We found that spiders, regardless of their developmental speed, behaved consistently in most of the tests. [...] The repeatability of activity was assessed using the R package ‘rptR’ [...] In order to test whether activity is rank order repeatable, we used Kendall's coefficient of concordance (also known as Kendall's W) as well. The reason of this was that by doing so one might see if individuals are consistent in their activity even if there is shift in their mean behaviour over ontogeny (Gyuris et al., 2012). [...] spiders were consistent in their behaviour across time in many of the behaviours. The exceptions were activity in the first test session, willingness to attack small artificial prey (also in the first test session), and in the second test session the latencies before catching prey and emergence from shelter. For activity in the first test session we got contradictory results between rank- and LMMbased analyses. Activity was repeatable according to the Kendall's coefficient of concordance, but not the LMM, probably because of the small sample size. As for the latencies before catching prey and emerging from shelter, it seems that those individuals that caught prey or emerged made their decisions in the first few seconds of the tests, which resulted in relatively large within-individual variances in the latency values, and thus statistically nonrepeatable measures of behaviour. Although individuals were consistent in their willingness to attack large artificial prey (in the first test session) and living prey (in the second test session), the probability of attacking small artificial prey (first test session) did not show significant repeatability.</t>
   </si>
   <si>
@@ -1935,9 +1908,6 @@
     <t>Both individual activity mesocosm (r±1 SE=0.231±0.081, 95% confidence interval (CI) 0.068–0.386, p=0.002; Fig. 1a) and RMR (r±1 SE=0.533±0.148, 95 % CI 0.227–0.838, p= 0.005; Fig. 1b) were repeatable over time, indicating temporal consistency in these traits. [...] Furthermore, in line with other studies of CIDs in massspecific metabolic rate (reviewed in White et al. 2013), our data indicate that mass-specific crab RMR is a temporally consistent trait at the individual level.</t>
   </si>
   <si>
-    <t>Individual variation in activitymesocosm and RMR was repeatable over time [...] We first tested for CIDs in crab activitymesocosm and RMR by measuring the repeatability (i.e., proportion of phenotypic variation due to between-individual variation) of these traits [...] We quantified the repeatability of P. herbstii RMR to examine CIDs in the energetic requirements of crabs [...] We analyzed the repeatability of activitymesocosm and RMR using the methods of Nakagawa and Schlereth (2010) and the associated rptR package in the statistical software R (R Core Team 2012). Repeatability is the proportion of total phenotypic variation due to between-subject, as opposed to within-subject variation (Lessells and Boag 1987;Bell et al. 2009). [...] Both individual activity mesocosm (r±1 SE=0.231±0.081, 95% confidence interval (CI) 0.068–0.386, p=0.002; Fig. 1a) and RMR (r±1 SE=0.533±0.148, 95 % CI 0.227–0.838, p= 0.005; Fig. 1b) were repeatable over time, indicating temporal consistency in these traits. [...] Furthermore, in line with other studies of CIDs in massspecific metabolic rate (reviewed in White et al. 2013), our data indicate that mass-specific crab RMR is a temporally consistent trait at the individual level. [...] Thus, support for an allocation model in our study is unique in that activity varied naturally among individual crabs, and this variation in individual activity was consistent over time (i.e., a behavioral type).</t>
-  </si>
-  <si>
     <t>Repeatability (conditional on fixed effects) was then calculated as the intraclass correlation, R = VI/(VI + VR), where VI is the among-individual variance and VR is the residual variance (Nakagawa &amp; Schielzeth, 2010). [...] While whole animal metabolic rate shows significant among-individual variation (R = 0.27 (0.11), χ2 0,1 = 8.031, p = 0.002) [...] All observed behaviours tested were repeatable, consistent with the presence of underlying personality variation, and growth rate also varied significantly among-fish over the experimental period. [...] Mass-specific RMR is sometimes expected to exhibit greater variation within individuals than SMR (due to uncontrolled activity during measurement of the latter), but nonetheless is often characterised by more moderate (R = 0.3–0.6) repeatability (Marras et al., 2010; Killen et al., 2011, 2014). We note of course that measurement error could be a non-trivial source of within fish variation, and inadequate precision of respirometers can cause low repeatability of metabolic traits (Nespolo &amp; Franco, 2007; Careau et al., 2008). Nonetheless, we feel this is unlikely to explain the complete absence of detectable VI here.</t>
   </si>
   <si>
@@ -1956,9 +1926,6 @@
     <t>Authors generally interpret repeatability as within but then, at the end, provide a couple of sentences highlighting the importance of both within and between individual variance when estimating repetability. Nonetheless, I thought that setting the interpretation of repetability to within reflected better how repeatability was generally interpreted in the paper.</t>
   </si>
   <si>
-    <t>The patterns of seed management were also extraordinarily variable between individuals and very repeatable within individuals across the scent treatment. For example, more than 75% of variation in seed dispersal distances and more than 80% of variation in dispersal effort (Pweight of seeds moved   distance moved) were explained by consistent differences between individuals. Overall, more than 87% of variance in activity in seed management trials was explained by consistent individual differences.</t>
-  </si>
-  <si>
     <t>The aim of this study was to analyse the individual variation and consistency in behaviour of scatter-hoarding rodents within a population. [...] We compared the variance and consistency in behaviours and acorn management due to individual differences with that due to manipulation, using genet scents, of the perceived predation risk. Genet scents reduced the activity (i.e. time out of the refuge) in all wood mice, but the differences and consistency in activity between individuals accounted for most of the variance. Also, mice showed different and consistent stress or relaxed behaviours. Most of the variance in seed management variables, such as dispersal distance and seed size selection, was explained by consistent differences between individuals across scent treatments. [...] We analysed the differences in behaviour between individuals, and the consistency within individuals across treatments, with a model that estimated the components of variance, with the ‘individual rodent’ as a random factor and ‘scent treatment’ (i.e. control, predator and control after predator) as a fixed factor.</t>
   </si>
   <si>
@@ -1995,15 +1962,6 @@
     <t>The individual behavioral consistency of all three measures in the 51 tagged individuals was high, as indicated by the individual repeatability estimates for visits per bout [...] Consistent with our observations from the laboratory, the wild G. commissarisi in this study exhibited individual behavioral consistency in the number of visits per bout they made to a patch of artificial flowers, their mean visit duration, and the number of different flowers they visited. The individual behavioral consistency of the three parameters could not be explained by their interdependence within a full domain-general syndrome</t>
   </si>
   <si>
-    <t>We considered three measures of an individual’s behaviour thatwere consistent over time [...] suggesting that pheasant chicks exhibit at least two distinct and unrelated sets of consis-tent behaviours across contexts, indicating two distinct personalitytraits.</t>
-  </si>
-  <si>
-    <t>Individuals were highly repeatable in the order in which theyentered the test arena across sessions (r = 0.34 ± 0.03; P &lt; 0.001;intra-class correlation coefficient = 0.95; P &lt; 0.01). [...] Each individual also showed repeatable latenciesto acquire the baseline worm across sessions (r = 0.15 ± 0.02;P &lt; 0.001; intra-class correlation coefficient = 0.87; P &lt; 0.001). [...] We considered three measures of an individual’s behaviour thatwere consistent over time [...] suggesting that pheasant chicks exhibit at least two distinct and unrelated sets of consis-tent behaviours across contexts, indicating two distinct personalitytraits. [...] our measure of test order may be consideredanalogous to previous accounts of competitive ability, which werealso found to be repeatable within individuals across time</t>
-  </si>
-  <si>
-    <t>To test for significant among-individual variation (i.e., personality) within each treatment and to test whether males from both treatments differed in this variation, we fitted another LMM [...] Because we scaled the total variance to 1 within each treatment, estimates for Vamong equal the behavioral repeatability, that is, the proportion of total variation that can be attributed to amongindividual differences in repeated measures data [...] Males differed consistently in their individual activity levels in both SCI treatments as indicated by significant deviation of Vamong (repeatability) from zero (Table 1a; Figure 2b,c). [...] Males differed consistently in their individual time to recover after a simulated predator attack as evidenced by significant deviation of Vamong (repeatability) from zero (Table 1b; Figure 2e,f). [...] Although males from both SCI treatments differed consistently in boldness and activity levels</t>
-  </si>
-  <si>
     <t>Authors compared groups in within- and among-individual variance - also in repeatability, but did not provide a specific interpretation of such comparison</t>
   </si>
   <si>
@@ -2013,9 +1971,6 @@
     <t>To establish which variables showed repeatable differences between individuals, and therefore constitute meaningful measures of intraspecific behavioural divergence in this species [...] To further characterize trait consistency, the intraclass correlation coefficient of each variable was calculated (ICC package;Wolak, Fairbairn, &amp; Paulsen, 2012). To focus subsequent analysis on divergence in variables that can be characterized as consistent phenotypic differences in behaviour, i.e. temperament traits, only significantly repeatable variables were included in statistical analysis of behavioural differences associated with habitat, sex and body length. [...] Repeatability, demonstrating consistent differences between desert gobies in behavioural responses within these assays, was significant in four variables (Table 2) [...] Desert gobies showed consistent within-species differences in behaviour on multiple axes,</t>
   </si>
   <si>
-    <t>Repeatability also measured as a correlation between individual behaviour measured at two different times. repeatability_consist_predict assigned as yes because that is how I interpret what is written in repeatability_consist_predict_context</t>
-  </si>
-  <si>
     <t xml:space="preserve"> NA</t>
   </si>
   <si>
@@ -2037,9 +1992,6 @@
     <t>Social connectedness meets the criteria for animal personality over time and across an environmental gradient, while both individual male and female elk showed consistent responses to changes in population density, although there was little variation in how individuals responded to changes in density.</t>
   </si>
   <si>
-    <t>Authors study both random intercept and random slopes, and generally refer to repeatability as both, however, there is at least once where repeatability is referred to as consistency.</t>
-  </si>
-  <si>
     <t>Lizards showed significant consistency within both behaviours, implying the presence of activity and risk-taking personalities. [...] Because both activity and risk-taking were repeatable within individuals across assays (see Results), we could use individual-specific estimates of these behaviours as traits reliably reflecting some aspects of an individual property. [...] We found that activity and risk-taking are both repeatable within individuals. The repeatability of behaviour is generally around 0.3–0.4 (Bell et al. 2009). Hence, the behavioural consistency of I. cyreni’s activity (r = 0.68) is high, while the consistency of risk-taking was rather low (r = 0.22). This adds to the slowly accumulating literature of reptilian behavioural consistency,</t>
   </si>
   <si>
@@ -2088,13 +2040,64 @@
     <t>Using doubly hierarchical-generalized linear models to analyse longitudinal data on startle responses, we show that hermit crabs vary both in their mean response durations and in the consistency of their behaviour. Individual consistency was unrelated to haemocyanin concentration or spermatophore size, but mean startle response duration increased with spermatophore size. [...] The random effects components of the mean model provide strong evidence for variation on the mean startle response duration among individuals that is not explained by the covariates in the model (table 1). This effect denotes significant repeatability in startle response duration. [...] As in previous studies, the data clearly show that hermit crabs exhibit animal personality in terms not only of consistent among-individual differences in mean level behaviour, but also in terms of significant among-individual differences in IIV.</t>
   </si>
   <si>
-    <t>The definition in the results suggest among but the start of the discussion suggest both.</t>
-  </si>
-  <si>
     <t>Females showed substantial inter-individual variation in how often they visited the different compartments in total during the two test days (mean ± SD = 1168 ± 984 visits, range 29–5112) and this behaviour was highly repeatable between test days [...] We also observed consistent inter-individual differences in activity and total number of visits (which might indicate different mate sampling behaviour),</t>
   </si>
   <si>
-    <t>Repeatability (stability/consistency) measured as a correlation between individual behaviour measured at two different times. In the discussion the mention consistent inter-individual differences, but I was not sure whether that refer to repeatability, and therefore, I keep the interpretation of repeatability as within</t>
+    <t>Repeatabilities were estimated as the intraclass coefficient at the individual level from [a model with] individuals' identities and cohort as random effects. [...] interindividual variation in exploration remained consistent across time and contexts. Thus, our test identified the well-known fast-slow exploration continuum, with some individuals consistently exploring both space and objects more than others. [...] We also need to assess how repeatable the measures are across time, which is a prerequisite for classifying the behaviour as a personality trait.</t>
+  </si>
+  <si>
+    <t>We tested whether changing labile components of individual state affected (i) behavioural consistency (the degree of between-individual difference) and (ii) behavioural type (mean behaviour) [...] We suggest that behavioural consistency is—on some level—affected by short-term ecological conditions in the studied population of adult male I. cyreni during the mating season. Hence, environmental conditions are likely responsible not only for the long-term development, but also for the short-term maintenance of individual behavioural variation. [...] As our behavioural assays covered an 8-day interval, we cannot claim that we report ‘true’ personalities that are consistent over long periods. [...] By showing that differences in environmental conditions cannot only shift the mean behaviour in animal groups during a short timeframe, but it might affect the level of between-individual variation too, we demonstrated the liability of behavioural consistency.</t>
+  </si>
+  <si>
+    <t>Authors define behavioural consistency as the degree of between-individual difference, and that is why repeatability_consist_predict was assigned as no</t>
+  </si>
+  <si>
+    <t>We found that individual differences in behavior were overall repeatable over ontogeny (i.e., personality was manifested). [...] Since we were interested in testing whether personality was manifested in genetically similar mosquitofish, we used the resulting among-individual and within-individual variance estimates from the LMMs described above to estimate the overall repeatability of each behavioral trait over fish ontogeny (Nakagawa and Schielzeth 2010; Dingemanse and Dochtermann 2013). Repeatability represents the proportion of behavioral variation attributable to consistent differences among individuals (Dingemanse and Dochtermann 2013). [...] To test whether the within- and the among-individual variance for a given behavioral trait increased or decreased over the ontogeny, we estimated both within- and among-individual variances for each behavior at each stage by using a MCMC sampling method [...] Across the entire experimental campaign, we detected personality differences among fish for each of the four behavioral traits measured, suggesting that individual differences in behavior were overall repeatable over the ontogeny of mosquitofish (Table 1). Nevertheless, the overall repeatability of fish behavior across the ontogeny was low (Table 1). [...] Furthermore, we observed a significant decline in the within-individual behavioral variance over ontogeny that was consistent to all behavioral traits for which personality was detected (Table 3; Fig. 4), whereas the among-individual variance did not vary with fish age for any trait (Table 3; Fig. 4).</t>
+  </si>
+  <si>
+    <t>repeatability_consist_predict assigned as no because temporal consistency seems to refer to consistency in differences according to the repeatability context</t>
+  </si>
+  <si>
+    <t>To include a standardised metric of behavioural consistency, and therefore personality, and give greater confidence to other interpretations, we calculated repeatability for each trait (latency to explore, latency to feed and correct food patch choice) as the ratio of between-individual variance (Vind) over the sum of Vind and the residual variance (Ve) from the random regression models (both within the solitary foraging context and across contexts)</t>
+  </si>
+  <si>
+    <t>First, we ran univariate models to calculate repeatability of behavioural traits. To do so, we decomposed the variance into within-individual (VW) and among-individual (VA) components, and repeatability (r) was calculated as VA/VA+VW . [...] Differences in personality may reflect genetic differences, phenotypic plasticity or flexibility (changes in behaviour resulting from environmental change), or all of these [...] Behavioural traits measured in the open field were repeatable (Table 1) and thus we can conclude that individual Siberian hamsters have different personalities, although these differences did not correlate with differences in winter phenotype.</t>
+  </si>
+  <si>
+    <t>there were consistent individual differences in cortisol release rate over time, with some individuals consistently releasing more cortisol than others across the two sampling periods (repeatability of sample average, R = 0.6159 [0.2252, 0.9218], n = 10, Fig. 2b). [...] There were consistent individual differences in boldness across the four measurements (R = 0.4980 [0.0817, 0.8244], n = 10, Fig. 3a). [...] We observed strong inter-individual variation among wild-caught individual sticklebacks from a natural population [...] For example, some sticklebacks were consistently more bold than others toward a model predator. [...] Additionally, we also observed that some individual sticklebacks were consistently morestress reactive than others.</t>
+  </si>
+  <si>
+    <t>repeatability_consist_predict is difficult to assign in this case, but think it is closer to no than yes, and assigned it as such</t>
+  </si>
+  <si>
+    <t>We found that spiders, regardless of their developmental speed, behaved consistently in most of the tests. [...] The repeatability of activity was assessed using the R package ‘rptR’ [...] In order to test whether activity is rank order repeatable, we used Kendall's coefficient of concordance (also known as Kendall's W) as well. The reason of this was that by doing so one might see if individuals are consistent in their activity even if there is shift in their mean behaviour over ontogeny (Gyuris et al., 2012). [...] spiders were consistent in their behaviour across time in many of the behaviours. The exceptions were activity in the first test session, willingness to attack small artificial prey (also in the first test session), and in the second test session the latencies before catching prey and emergence from shelter. For activity in the first test session we got contradictory results between rank- and LMM-based analyses. Activity was repeatable according to the Kendall's coefficient of concordance, but not the LMM, probably because of the small sample size. As for the latencies before catching prey and emerging from shelter, it seems that those individuals that caught prey or emerged made their decisions in the first few seconds of the tests, which resulted in relatively large within-individual variances in the latency values, and thus statistically nonrepeatable measures of behaviour. Although individuals were consistent in their willingness to attack large artificial prey (in the first test session) and living prey (in the second test session), the probability of attacking small artificial prey (first test session) did not show significant repeatability.</t>
+  </si>
+  <si>
+    <t>Individual variation in activity mesocosm and RMR was repeatable over time [...] We first tested for CIDs in crab activity mesocosm and RMR by measuring the repeatability (i.e., proportion of phenotypic variation due to between-individual variation) of these traits [...] We quantified the repeatability of P. herbstii RMR to examine CIDs in the energetic requirements of crabs [...] We analyzed the repeatability of activity mesocosm and RMR using the methods of Nakagawa and Schlereth (2010) and the associated rptR package in the statistical software R (R Core Team 2012). Repeatability is the proportion of total phenotypic variation due to between-subject, as opposed to within-subject variation (Lessells and Boag 1987;Bell et al. 2009). [...] Both individual activity mesocosm (r±1 SE=0.231±0.081, 95% confidence interval (CI) 0.068–0.386, p=0.002; Fig. 1a) and RMR (r±1 SE=0.533±0.148, 95 % CI 0.227–0.838, p= 0.005; Fig. 1b) were repeatable over time, indicating temporal consistency in these traits. [...] Furthermore, in line with other studies of CIDs in massspecific metabolic rate (reviewed in White et al. 2013), our data indicate that mass-specific crab RMR is a temporally consistent trait at the individual level. [...] Thus, support for an allocation model in our study is unique in that activity varied naturally among individual crabs, and this variation in individual activity was consistent over time (i.e., a behavioral type).</t>
+  </si>
+  <si>
+    <t>The patterns of seed management were also extraordinarily variable between individuals and very repeatable within individuals across the scent treatment. For example, more than 75% of variation in seed dispersal distances and more than 80% of variation in dispersal effort (Pweight of seeds moved distance moved) were explained by consistent differences between individuals. Overall, more than 87% of variance in activity in seed management trials was explained by consistent individual differences.</t>
+  </si>
+  <si>
+    <t>Individuals were highly repeatable in the order in which they entered the test arena across sessions (r = 0.34 ± 0.03; P &lt; 0.001; intra-class correlation coefficient = 0.95; P &lt; 0.01). [...] Each individual also showed repeatable latencies to acquire the baseline worm across sessions (r = 0.15 ± 0.02;P &lt; 0.001; intra-class correlation coefficient = 0.87; P &lt; 0.001). [...] We considered three measures of an individual’s behaviour that were consistent over time [...] suggesting that pheasant chicks exhibit at least two distinct and unrelated sets of consistent behaviours across contexts, indicating two distinct personality traits. [...] our measure of test order may be considered analogous to previous accounts of competitive ability, which were also found to be repeatable within individuals across time</t>
+  </si>
+  <si>
+    <t>We considered three measures of an individual’s behaviour that were consistent over time [...] suggesting that pheasant chicks exhibit at least two distinct and unrelated sets of consistent behaviours across contexts, indicating two distinct personality traits.</t>
+  </si>
+  <si>
+    <t>To test for significant among-individual variation (i.e., personality) within each treatment and to test whether males from both treatments differed in this variation, we fitted another LMM [...] Because we scaled the total variance to 1 within each treatment, estimates for Vamong equal the behavioral repeatability, that is, the proportion of total variation that can be attributed to among individual differences in repeated measures data [...] Males differed consistently in their individual activity levels in both SCI treatments as indicated by significant deviation of Vamong (repeatability) from zero (Table 1a; Figure 2b,c). [...] Males differed consistently in their individual time to recover after a simulated predator attack as evidenced by significant deviation of Vamong (repeatability) from zero (Table 1b; Figure 2e,f). [...] Although males from both SCI treatments differed consistently in boldness and activity levels</t>
+  </si>
+  <si>
+    <t>Repeatability also measured as a correlation between individual behaviour measured at two different times. repeatability_consist_predict assigned as no because it is unclear whether it refers to individual consistency or, instead, as it seems the case here, to consistent differences. Nonetheless, unclear case.</t>
+  </si>
+  <si>
+    <t>Authors study both random intercept and random slopes, and generally refer to repeatability as both, however, repeatability is also referred to as consistency.</t>
+  </si>
+  <si>
+    <t>The definition in the results suggest among but the start of the discussion suggest both. I leaned towards both for the interpretation.</t>
+  </si>
+  <si>
+    <t>Repeatability (stability/consistency)also measured as a correlation between individual behaviour measured at two different times. In the discussion the mention consistent inter-individual differences, but I was not sure whether that refer to repeatability, and therefore, I keep the interpretation of repeatability as within</t>
   </si>
 </sst>
 </file>
@@ -2142,7 +2145,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -2152,6 +2155,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2450,8 +2454,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AG75"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="T52" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="Z82" sqref="Z82"/>
+    <sheetView tabSelected="1" topLeftCell="W1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="Y16" sqref="Y16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2662,7 +2667,7 @@
         <v>581</v>
       </c>
       <c r="AF2" s="3" t="s">
-        <v>599</v>
+        <v>596</v>
       </c>
       <c r="AG2" s="3" t="s">
         <v>46</v>
@@ -2733,7 +2738,7 @@
         <v>584</v>
       </c>
       <c r="Y3" s="3" t="s">
-        <v>585</v>
+        <v>674</v>
       </c>
       <c r="Z3" s="3" t="s">
         <v>582</v>
@@ -2757,98 +2762,98 @@
         <v>46</v>
       </c>
     </row>
-    <row r="4" spans="1:33" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="5" t="s">
+    <row r="4" spans="1:33" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="B4" s="5" t="s">
+      <c r="B4" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="C4" s="5" t="s">
+      <c r="C4" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="D4" s="5">
+      <c r="D4" s="4">
         <v>2015</v>
       </c>
-      <c r="E4" s="5">
-        <v>1</v>
-      </c>
-      <c r="F4" s="5">
-        <v>1</v>
-      </c>
-      <c r="G4" s="5" t="s">
+      <c r="E4" s="4">
+        <v>1</v>
+      </c>
+      <c r="F4" s="4">
+        <v>1</v>
+      </c>
+      <c r="G4" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="H4" s="5" t="s">
+      <c r="H4" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="I4" s="5">
+      <c r="I4" s="4">
         <v>26</v>
       </c>
-      <c r="J4" s="5">
+      <c r="J4" s="4">
         <v>6</v>
       </c>
-      <c r="K4" s="5" t="s">
+      <c r="K4" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="L4" s="5" t="s">
+      <c r="L4" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="M4" s="5" t="s">
+      <c r="M4" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="O4" s="5" t="s">
+      <c r="O4" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="Q4" s="5" t="s">
+      <c r="Q4" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="R4" s="5" t="s">
+      <c r="R4" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="S4" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="T4" s="5" t="s">
-        <v>581</v>
-      </c>
-      <c r="U4" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="V4" s="5" t="s">
-        <v>581</v>
-      </c>
-      <c r="W4" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="X4" s="5" t="s">
+      <c r="S4" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="T4" s="4" t="s">
+        <v>581</v>
+      </c>
+      <c r="U4" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="V4" s="4" t="s">
+        <v>581</v>
+      </c>
+      <c r="W4" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="X4" s="4" t="s">
+        <v>585</v>
+      </c>
+      <c r="Y4" s="4" t="s">
+        <v>586</v>
+      </c>
+      <c r="Z4" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="AA4" s="4" t="s">
         <v>587</v>
       </c>
-      <c r="Y4" s="5" t="s">
+      <c r="AB4" s="4" t="s">
+        <v>582</v>
+      </c>
+      <c r="AC4" s="4" t="s">
+        <v>581</v>
+      </c>
+      <c r="AD4" s="4" t="s">
+        <v>581</v>
+      </c>
+      <c r="AE4" s="4" t="s">
+        <v>582</v>
+      </c>
+      <c r="AF4" s="4" t="s">
         <v>588</v>
       </c>
-      <c r="Z4" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="AA4" s="5" t="s">
-        <v>589</v>
-      </c>
-      <c r="AB4" s="5" t="s">
-        <v>582</v>
-      </c>
-      <c r="AC4" s="5" t="s">
-        <v>581</v>
-      </c>
-      <c r="AD4" s="5" t="s">
-        <v>581</v>
-      </c>
-      <c r="AE4" s="5" t="s">
-        <v>582</v>
-      </c>
-      <c r="AF4" s="5" t="s">
-        <v>590</v>
-      </c>
-      <c r="AG4" s="5" t="s">
+      <c r="AG4" s="4" t="s">
         <v>46</v>
       </c>
     </row>
@@ -2917,13 +2922,13 @@
         <v>584</v>
       </c>
       <c r="Y5" s="3" t="s">
-        <v>592</v>
+        <v>590</v>
       </c>
       <c r="Z5" s="3" t="s">
         <v>44</v>
       </c>
       <c r="AA5" s="3" t="s">
-        <v>593</v>
+        <v>591</v>
       </c>
       <c r="AB5" s="3" t="s">
         <v>582</v>
@@ -2938,7 +2943,7 @@
         <v>582</v>
       </c>
       <c r="AF5" s="3" t="s">
-        <v>591</v>
+        <v>589</v>
       </c>
       <c r="AG5" s="3" t="s">
         <v>46</v>
@@ -3033,101 +3038,98 @@
         <v>581</v>
       </c>
       <c r="AF6" s="3" t="s">
-        <v>594</v>
+        <v>592</v>
       </c>
       <c r="AG6" s="3" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="7" spans="1:33" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="5" t="s">
+    <row r="7" spans="1:33" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="B7" s="5" t="s">
+      <c r="B7" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="C7" s="5" t="s">
+      <c r="C7" s="4" t="s">
         <v>84</v>
       </c>
-      <c r="D7" s="5">
+      <c r="D7" s="4">
         <v>2017</v>
       </c>
-      <c r="E7" s="5">
-        <v>1</v>
-      </c>
-      <c r="F7" s="5">
-        <v>1</v>
-      </c>
-      <c r="G7" s="5" t="s">
+      <c r="E7" s="4">
+        <v>1</v>
+      </c>
+      <c r="F7" s="4">
+        <v>1</v>
+      </c>
+      <c r="G7" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="H7" s="5" t="s">
+      <c r="H7" s="4" t="s">
         <v>86</v>
       </c>
-      <c r="I7" s="5">
+      <c r="I7" s="4">
         <v>284</v>
       </c>
-      <c r="J7" s="5">
+      <c r="J7" s="4">
         <v>1868</v>
       </c>
-      <c r="L7" s="5" t="s">
+      <c r="L7" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="M7" s="5" t="s">
+      <c r="M7" s="4" t="s">
         <v>88</v>
       </c>
-      <c r="O7" s="5" t="s">
+      <c r="O7" s="4" t="s">
         <v>89</v>
       </c>
-      <c r="Q7" s="5" t="s">
+      <c r="Q7" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="R7" s="5" t="s">
+      <c r="R7" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="S7" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="T7" s="5" t="s">
-        <v>581</v>
-      </c>
-      <c r="U7" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="V7" s="5" t="s">
-        <v>581</v>
-      </c>
-      <c r="W7" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="X7" s="5" t="s">
-        <v>583</v>
-      </c>
-      <c r="Y7" s="5" t="s">
-        <v>595</v>
-      </c>
-      <c r="Z7" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="AA7" s="5" t="s">
-        <v>597</v>
-      </c>
-      <c r="AB7" s="5" t="s">
-        <v>582</v>
-      </c>
-      <c r="AC7" s="5" t="s">
-        <v>581</v>
-      </c>
-      <c r="AD7" s="5" t="s">
-        <v>581</v>
-      </c>
-      <c r="AE7" s="5" t="s">
-        <v>582</v>
-      </c>
-      <c r="AF7" s="5" t="s">
-        <v>596</v>
-      </c>
-      <c r="AG7" s="5" t="s">
+      <c r="S7" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="T7" s="4" t="s">
+        <v>581</v>
+      </c>
+      <c r="U7" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="V7" s="4" t="s">
+        <v>581</v>
+      </c>
+      <c r="W7" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="X7" s="4" t="s">
+        <v>584</v>
+      </c>
+      <c r="Y7" s="4" t="s">
+        <v>593</v>
+      </c>
+      <c r="Z7" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="AA7" s="4" t="s">
+        <v>594</v>
+      </c>
+      <c r="AB7" s="4" t="s">
+        <v>582</v>
+      </c>
+      <c r="AC7" s="4" t="s">
+        <v>581</v>
+      </c>
+      <c r="AD7" s="4" t="s">
+        <v>581</v>
+      </c>
+      <c r="AE7" s="4" t="s">
+        <v>582</v>
+      </c>
+      <c r="AG7" s="4" t="s">
         <v>46</v>
       </c>
     </row>
@@ -3196,7 +3198,7 @@
         <v>584</v>
       </c>
       <c r="Y8" s="3" t="s">
-        <v>598</v>
+        <v>595</v>
       </c>
       <c r="Z8" s="3" t="s">
         <v>582</v>
@@ -3312,7 +3314,7 @@
         <v>581</v>
       </c>
       <c r="AF9" s="3" t="s">
-        <v>605</v>
+        <v>602</v>
       </c>
       <c r="AG9" s="3" t="s">
         <v>46</v>
@@ -3380,7 +3382,7 @@
         <v>44</v>
       </c>
       <c r="X10" s="3" t="s">
-        <v>581</v>
+        <v>627</v>
       </c>
       <c r="Y10" s="3" t="s">
         <v>581</v>
@@ -3404,7 +3406,7 @@
         <v>582</v>
       </c>
       <c r="AF10" s="3" t="s">
-        <v>600</v>
+        <v>597</v>
       </c>
       <c r="AG10" s="3" t="s">
         <v>46</v>
@@ -3475,13 +3477,13 @@
         <v>583</v>
       </c>
       <c r="Y11" s="3" t="s">
-        <v>601</v>
+        <v>598</v>
       </c>
       <c r="Z11" s="3" t="s">
         <v>44</v>
       </c>
       <c r="AA11" s="3" t="s">
-        <v>602</v>
+        <v>599</v>
       </c>
       <c r="AB11" s="3" t="s">
         <v>582</v>
@@ -3570,7 +3572,7 @@
         <v>584</v>
       </c>
       <c r="Y12" s="3" t="s">
-        <v>603</v>
+        <v>600</v>
       </c>
       <c r="Z12" s="3" t="s">
         <v>582</v>
@@ -3775,7 +3777,7 @@
         <v>581</v>
       </c>
       <c r="AF14" s="3" t="s">
-        <v>604</v>
+        <v>601</v>
       </c>
       <c r="AG14" s="3" t="s">
         <v>46</v>
@@ -3867,101 +3869,101 @@
         <v>581</v>
       </c>
       <c r="AF15" s="3" t="s">
-        <v>604</v>
+        <v>601</v>
       </c>
       <c r="AG15" s="3" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="16" spans="1:33" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="5" t="s">
+    <row r="16" spans="1:33" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="4" t="s">
         <v>149</v>
       </c>
-      <c r="B16" s="5" t="s">
+      <c r="B16" s="4" t="s">
         <v>150</v>
       </c>
-      <c r="C16" s="5" t="s">
+      <c r="C16" s="4" t="s">
         <v>151</v>
       </c>
-      <c r="D16" s="5">
+      <c r="D16" s="4">
         <v>2017</v>
       </c>
-      <c r="E16" s="5">
-        <v>1</v>
-      </c>
-      <c r="F16" s="5">
-        <v>1</v>
-      </c>
-      <c r="G16" s="5" t="s">
+      <c r="E16" s="4">
+        <v>1</v>
+      </c>
+      <c r="F16" s="4">
+        <v>1</v>
+      </c>
+      <c r="G16" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="H16" s="5" t="s">
+      <c r="H16" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="I16" s="5">
+      <c r="I16" s="4">
         <v>71</v>
       </c>
-      <c r="J16" s="5">
-        <v>1</v>
-      </c>
-      <c r="L16" s="5" t="s">
+      <c r="J16" s="4">
+        <v>1</v>
+      </c>
+      <c r="L16" s="4" t="s">
         <v>152</v>
       </c>
-      <c r="M16" s="5" t="s">
+      <c r="M16" s="4" t="s">
         <v>153</v>
       </c>
-      <c r="O16" s="5" t="s">
+      <c r="O16" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="Q16" s="5" t="s">
+      <c r="Q16" s="4" t="s">
         <v>154</v>
       </c>
-      <c r="R16" s="5" t="s">
+      <c r="R16" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="S16" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="T16" s="5" t="s">
-        <v>581</v>
-      </c>
-      <c r="U16" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="V16" s="5" t="s">
-        <v>581</v>
-      </c>
-      <c r="W16" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="X16" s="5" t="s">
-        <v>609</v>
-      </c>
-      <c r="Y16" s="5" t="s">
-        <v>610</v>
-      </c>
-      <c r="Z16" s="5" t="s">
-        <v>606</v>
-      </c>
-      <c r="AA16" s="5" t="s">
-        <v>608</v>
-      </c>
-      <c r="AB16" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="AC16" s="5" t="s">
-        <v>586</v>
-      </c>
-      <c r="AD16" s="5" t="s">
-        <v>607</v>
-      </c>
-      <c r="AE16" s="5" t="s">
-        <v>582</v>
-      </c>
-      <c r="AF16" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="AG16" s="5" t="s">
+      <c r="S16" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="T16" s="4" t="s">
+        <v>581</v>
+      </c>
+      <c r="U16" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="V16" s="4" t="s">
+        <v>581</v>
+      </c>
+      <c r="W16" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="X16" s="4" t="s">
+        <v>584</v>
+      </c>
+      <c r="Y16" s="4" t="s">
+        <v>675</v>
+      </c>
+      <c r="Z16" s="4" t="s">
+        <v>582</v>
+      </c>
+      <c r="AA16" s="4" t="s">
+        <v>604</v>
+      </c>
+      <c r="AB16" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="AC16" s="4" t="s">
+        <v>585</v>
+      </c>
+      <c r="AD16" s="4" t="s">
+        <v>603</v>
+      </c>
+      <c r="AE16" s="4" t="s">
+        <v>582</v>
+      </c>
+      <c r="AF16" s="4" t="s">
+        <v>676</v>
+      </c>
+      <c r="AG16" s="4" t="s">
         <v>46</v>
       </c>
     </row>
@@ -4057,98 +4059,98 @@
         <v>46</v>
       </c>
     </row>
-    <row r="18" spans="1:33" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="5" t="s">
+    <row r="18" spans="1:33" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="4" t="s">
         <v>162</v>
       </c>
-      <c r="B18" s="5" t="s">
+      <c r="B18" s="4" t="s">
         <v>163</v>
       </c>
-      <c r="C18" s="5" t="s">
+      <c r="C18" s="4" t="s">
         <v>164</v>
       </c>
-      <c r="D18" s="5">
+      <c r="D18" s="4">
         <v>2015</v>
       </c>
-      <c r="E18" s="5">
-        <v>1</v>
-      </c>
-      <c r="F18" s="5">
-        <v>1</v>
-      </c>
-      <c r="G18" s="5" t="s">
+      <c r="E18" s="4">
+        <v>1</v>
+      </c>
+      <c r="F18" s="4">
+        <v>1</v>
+      </c>
+      <c r="G18" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="H18" s="5" t="s">
+      <c r="H18" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="I18" s="5">
+      <c r="I18" s="4">
         <v>69</v>
       </c>
-      <c r="J18" s="5">
+      <c r="J18" s="4">
         <v>6</v>
       </c>
-      <c r="K18" s="5" t="s">
+      <c r="K18" s="4" t="s">
         <v>165</v>
       </c>
-      <c r="L18" s="5" t="s">
+      <c r="L18" s="4" t="s">
         <v>166</v>
       </c>
-      <c r="M18" s="5" t="s">
+      <c r="M18" s="4" t="s">
         <v>167</v>
       </c>
-      <c r="O18" s="5" t="s">
+      <c r="O18" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="Q18" s="5" t="s">
+      <c r="Q18" s="4" t="s">
         <v>168</v>
       </c>
-      <c r="R18" s="5" t="s">
+      <c r="R18" s="4" t="s">
         <v>127</v>
       </c>
-      <c r="S18" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="T18" s="5" t="s">
-        <v>581</v>
-      </c>
-      <c r="U18" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="V18" s="5" t="s">
-        <v>581</v>
-      </c>
-      <c r="W18" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="X18" s="5" t="s">
-        <v>583</v>
-      </c>
-      <c r="Y18" s="5" t="s">
-        <v>611</v>
-      </c>
-      <c r="Z18" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="AA18" s="5" t="s">
-        <v>611</v>
-      </c>
-      <c r="AB18" s="5" t="s">
-        <v>582</v>
-      </c>
-      <c r="AC18" s="5" t="s">
-        <v>581</v>
-      </c>
-      <c r="AD18" s="5" t="s">
-        <v>581</v>
-      </c>
-      <c r="AE18" s="5" t="s">
-        <v>582</v>
-      </c>
-      <c r="AF18" s="5" t="s">
-        <v>612</v>
-      </c>
-      <c r="AG18" s="5" t="s">
+      <c r="S18" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="T18" s="4" t="s">
+        <v>581</v>
+      </c>
+      <c r="U18" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="V18" s="4" t="s">
+        <v>581</v>
+      </c>
+      <c r="W18" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="X18" s="4" t="s">
+        <v>584</v>
+      </c>
+      <c r="Y18" s="4" t="s">
+        <v>605</v>
+      </c>
+      <c r="Z18" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="AA18" s="4" t="s">
+        <v>605</v>
+      </c>
+      <c r="AB18" s="4" t="s">
+        <v>582</v>
+      </c>
+      <c r="AC18" s="4" t="s">
+        <v>581</v>
+      </c>
+      <c r="AD18" s="4" t="s">
+        <v>581</v>
+      </c>
+      <c r="AE18" s="4" t="s">
+        <v>582</v>
+      </c>
+      <c r="AF18" s="4" t="s">
+        <v>606</v>
+      </c>
+      <c r="AG18" s="4" t="s">
         <v>46</v>
       </c>
     </row>
@@ -4217,10 +4219,10 @@
         <v>44</v>
       </c>
       <c r="X19" s="3" t="s">
-        <v>586</v>
+        <v>584</v>
       </c>
       <c r="Y19" s="3" t="s">
-        <v>613</v>
+        <v>607</v>
       </c>
       <c r="Z19" s="3" t="s">
         <v>582</v>
@@ -4315,13 +4317,13 @@
         <v>584</v>
       </c>
       <c r="Y20" s="3" t="s">
-        <v>614</v>
+        <v>608</v>
       </c>
       <c r="Z20" s="3" t="s">
         <v>44</v>
       </c>
       <c r="AA20" s="3" t="s">
-        <v>616</v>
+        <v>610</v>
       </c>
       <c r="AB20" s="3" t="s">
         <v>44</v>
@@ -4330,7 +4332,7 @@
         <v>583</v>
       </c>
       <c r="AD20" s="3" t="s">
-        <v>615</v>
+        <v>609</v>
       </c>
       <c r="AE20" s="3" t="s">
         <v>44</v>
@@ -4410,7 +4412,7 @@
         <v>584</v>
       </c>
       <c r="Y21" s="3" t="s">
-        <v>617</v>
+        <v>677</v>
       </c>
       <c r="Z21" s="3" t="s">
         <v>582</v>
@@ -4523,7 +4525,7 @@
         <v>581</v>
       </c>
       <c r="AF22" s="3" t="s">
-        <v>618</v>
+        <v>611</v>
       </c>
       <c r="AG22" s="3" t="s">
         <v>46</v>
@@ -4689,13 +4691,13 @@
         <v>584</v>
       </c>
       <c r="Y24" s="3" t="s">
-        <v>620</v>
+        <v>613</v>
       </c>
       <c r="Z24" s="3" t="s">
         <v>582</v>
       </c>
       <c r="AA24" s="3" t="s">
-        <v>619</v>
+        <v>612</v>
       </c>
       <c r="AB24" s="3" t="s">
         <v>582</v>
@@ -4710,196 +4712,196 @@
         <v>582</v>
       </c>
       <c r="AF24" s="3" t="s">
-        <v>45</v>
+        <v>678</v>
       </c>
       <c r="AG24" s="3" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="25" spans="1:33" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="5" t="s">
+    <row r="25" spans="1:33" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="4" t="s">
         <v>216</v>
       </c>
-      <c r="B25" s="5" t="s">
+      <c r="B25" s="4" t="s">
         <v>217</v>
       </c>
-      <c r="C25" s="5" t="s">
+      <c r="C25" s="4" t="s">
         <v>218</v>
       </c>
-      <c r="D25" s="5">
+      <c r="D25" s="4">
         <v>2017</v>
       </c>
-      <c r="E25" s="5">
-        <v>1</v>
-      </c>
-      <c r="F25" s="5">
-        <v>1</v>
-      </c>
-      <c r="G25" s="5" t="s">
+      <c r="E25" s="4">
+        <v>1</v>
+      </c>
+      <c r="F25" s="4">
+        <v>1</v>
+      </c>
+      <c r="G25" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="H25" s="5" t="s">
+      <c r="H25" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="I25" s="5">
+      <c r="I25" s="4">
         <v>123</v>
       </c>
-      <c r="K25" s="5" t="s">
+      <c r="K25" s="4" t="s">
         <v>219</v>
       </c>
-      <c r="L25" s="5" t="s">
+      <c r="L25" s="4" t="s">
         <v>220</v>
       </c>
-      <c r="M25" s="5" t="s">
+      <c r="M25" s="4" t="s">
         <v>221</v>
       </c>
-      <c r="O25" s="5" t="s">
+      <c r="O25" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="Q25" s="5" t="s">
+      <c r="Q25" s="4" t="s">
         <v>222</v>
       </c>
-      <c r="R25" s="5" t="s">
+      <c r="R25" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="S25" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="T25" s="5" t="s">
-        <v>581</v>
-      </c>
-      <c r="U25" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="V25" s="5" t="s">
-        <v>581</v>
-      </c>
-      <c r="W25" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="X25" s="5" t="s">
+      <c r="S25" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="T25" s="4" t="s">
+        <v>581</v>
+      </c>
+      <c r="U25" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="V25" s="4" t="s">
+        <v>581</v>
+      </c>
+      <c r="W25" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="X25" s="4" t="s">
         <v>583</v>
       </c>
-      <c r="Y25" s="5" t="s">
-        <v>624</v>
-      </c>
-      <c r="Z25" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="AA25" s="5" t="s">
-        <v>621</v>
-      </c>
-      <c r="AB25" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="AC25" s="5" t="s">
+      <c r="Y25" s="4" t="s">
+        <v>617</v>
+      </c>
+      <c r="Z25" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="AA25" s="4" t="s">
+        <v>614</v>
+      </c>
+      <c r="AB25" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="AC25" s="4" t="s">
         <v>583</v>
       </c>
-      <c r="AD25" s="5" t="s">
-        <v>623</v>
-      </c>
-      <c r="AE25" s="5" t="s">
-        <v>582</v>
-      </c>
-      <c r="AF25" s="5" t="s">
-        <v>622</v>
-      </c>
-      <c r="AG25" s="5" t="s">
+      <c r="AD25" s="4" t="s">
+        <v>616</v>
+      </c>
+      <c r="AE25" s="4" t="s">
+        <v>582</v>
+      </c>
+      <c r="AF25" s="4" t="s">
+        <v>615</v>
+      </c>
+      <c r="AG25" s="4" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="26" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A26" s="3" t="s">
+    <row r="26" spans="1:33" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="9" t="s">
         <v>223</v>
       </c>
-      <c r="B26" s="3" t="s">
+      <c r="B26" s="9" t="s">
         <v>224</v>
       </c>
-      <c r="C26" s="3" t="s">
+      <c r="C26" s="9" t="s">
         <v>225</v>
       </c>
-      <c r="D26" s="3">
+      <c r="D26" s="9">
         <v>2016</v>
       </c>
-      <c r="E26" s="3">
-        <v>1</v>
-      </c>
-      <c r="F26" s="3">
-        <v>1</v>
-      </c>
-      <c r="G26" s="3" t="s">
+      <c r="E26" s="9">
+        <v>1</v>
+      </c>
+      <c r="F26" s="9">
+        <v>1</v>
+      </c>
+      <c r="G26" s="9" t="s">
         <v>68</v>
       </c>
-      <c r="H26" s="3" t="s">
+      <c r="H26" s="9" t="s">
         <v>69</v>
       </c>
-      <c r="I26" s="3">
+      <c r="I26" s="9">
         <v>70</v>
       </c>
-      <c r="J26" s="3">
+      <c r="J26" s="9">
         <v>11</v>
       </c>
-      <c r="K26" s="3" t="s">
+      <c r="K26" s="9" t="s">
         <v>226</v>
       </c>
-      <c r="L26" s="3" t="s">
+      <c r="L26" s="9" t="s">
         <v>227</v>
       </c>
-      <c r="M26" s="3" t="s">
+      <c r="M26" s="9" t="s">
         <v>228</v>
       </c>
-      <c r="O26" s="3" t="s">
+      <c r="O26" s="9" t="s">
         <v>72</v>
       </c>
-      <c r="Q26" s="3" t="s">
+      <c r="Q26" s="9" t="s">
         <v>229</v>
       </c>
-      <c r="R26" s="3" t="s">
+      <c r="R26" s="9" t="s">
         <v>127</v>
       </c>
-      <c r="S26" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="T26" s="3" t="s">
-        <v>581</v>
-      </c>
-      <c r="U26" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="V26" s="3" t="s">
-        <v>581</v>
-      </c>
-      <c r="W26" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="X26" s="3" t="s">
-        <v>584</v>
-      </c>
-      <c r="Y26" s="3" t="s">
-        <v>625</v>
-      </c>
-      <c r="Z26" s="3" t="s">
-        <v>582</v>
-      </c>
-      <c r="AA26" s="3" t="s">
-        <v>625</v>
-      </c>
-      <c r="AB26" s="3" t="s">
-        <v>582</v>
-      </c>
-      <c r="AC26" s="3" t="s">
-        <v>581</v>
-      </c>
-      <c r="AD26" s="3" t="s">
-        <v>581</v>
-      </c>
-      <c r="AE26" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="AF26" s="3" t="s">
-        <v>626</v>
-      </c>
-      <c r="AG26" s="3" t="s">
+      <c r="S26" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="T26" s="9" t="s">
+        <v>581</v>
+      </c>
+      <c r="U26" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="V26" s="9" t="s">
+        <v>581</v>
+      </c>
+      <c r="W26" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="X26" s="9" t="s">
+        <v>583</v>
+      </c>
+      <c r="Y26" s="9" t="s">
+        <v>679</v>
+      </c>
+      <c r="Z26" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="AA26" s="9" t="s">
+        <v>618</v>
+      </c>
+      <c r="AB26" s="9" t="s">
+        <v>582</v>
+      </c>
+      <c r="AC26" s="9" t="s">
+        <v>581</v>
+      </c>
+      <c r="AD26" s="9" t="s">
+        <v>581</v>
+      </c>
+      <c r="AE26" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="AF26" s="9" t="s">
+        <v>619</v>
+      </c>
+      <c r="AG26" s="9" t="s">
         <v>46</v>
       </c>
     </row>
@@ -5066,13 +5068,13 @@
         <v>584</v>
       </c>
       <c r="Y28" s="3" t="s">
-        <v>627</v>
+        <v>620</v>
       </c>
       <c r="Z28" s="3" t="s">
         <v>44</v>
       </c>
       <c r="AA28" s="3" t="s">
-        <v>628</v>
+        <v>621</v>
       </c>
       <c r="AB28" s="3" t="s">
         <v>582</v>
@@ -5253,7 +5255,7 @@
         <v>583</v>
       </c>
       <c r="Y30" s="4" t="s">
-        <v>630</v>
+        <v>623</v>
       </c>
       <c r="Z30" s="4" t="s">
         <v>582</v>
@@ -5274,7 +5276,7 @@
         <v>582</v>
       </c>
       <c r="AF30" s="4" t="s">
-        <v>629</v>
+        <v>622</v>
       </c>
       <c r="AG30" s="4" t="s">
         <v>46</v>
@@ -5369,7 +5371,7 @@
         <v>581</v>
       </c>
       <c r="AF31" s="3" t="s">
-        <v>604</v>
+        <v>601</v>
       </c>
       <c r="AG31" s="3" t="s">
         <v>46</v>
@@ -5440,7 +5442,7 @@
         <v>584</v>
       </c>
       <c r="Y32" s="3" t="s">
-        <v>631</v>
+        <v>680</v>
       </c>
       <c r="Z32" s="4" t="s">
         <v>582</v>
@@ -5532,13 +5534,13 @@
         <v>584</v>
       </c>
       <c r="Y33" s="3" t="s">
-        <v>632</v>
+        <v>681</v>
       </c>
       <c r="Z33" s="4" t="s">
         <v>582</v>
       </c>
-      <c r="AA33" s="4" t="s">
-        <v>581</v>
+      <c r="AA33" s="3" t="s">
+        <v>681</v>
       </c>
       <c r="AB33" s="4" t="s">
         <v>582</v>
@@ -5552,8 +5554,8 @@
       <c r="AE33" s="4" t="s">
         <v>582</v>
       </c>
-      <c r="AF33" s="3" t="s">
-        <v>45</v>
+      <c r="AF33" s="4" t="s">
+        <v>682</v>
       </c>
       <c r="AG33" s="3" t="s">
         <v>46</v>
@@ -5624,7 +5626,7 @@
         <v>584</v>
       </c>
       <c r="Y34" s="3" t="s">
-        <v>635</v>
+        <v>626</v>
       </c>
       <c r="Z34" s="4" t="s">
         <v>582</v>
@@ -5636,7 +5638,7 @@
         <v>44</v>
       </c>
       <c r="AC34" s="4" t="s">
-        <v>636</v>
+        <v>627</v>
       </c>
       <c r="AD34" s="4" t="s">
         <v>581</v>
@@ -5714,13 +5716,13 @@
         <v>583</v>
       </c>
       <c r="Y35" s="3" t="s">
-        <v>633</v>
+        <v>683</v>
       </c>
       <c r="Z35" s="4" t="s">
         <v>44</v>
       </c>
       <c r="AA35" s="3" t="s">
-        <v>633</v>
+        <v>624</v>
       </c>
       <c r="AB35" s="4" t="s">
         <v>582</v>
@@ -5735,7 +5737,7 @@
         <v>582</v>
       </c>
       <c r="AF35" s="4" t="s">
-        <v>634</v>
+        <v>625</v>
       </c>
       <c r="AG35" s="3" t="s">
         <v>46</v>
@@ -5901,16 +5903,16 @@
         <v>44</v>
       </c>
       <c r="X37" s="4" t="s">
-        <v>583</v>
+        <v>584</v>
       </c>
       <c r="Y37" s="3" t="s">
-        <v>638</v>
+        <v>684</v>
       </c>
       <c r="Z37" s="3" t="s">
         <v>44</v>
       </c>
       <c r="AA37" s="3" t="s">
-        <v>637</v>
+        <v>628</v>
       </c>
       <c r="AB37" s="4" t="s">
         <v>582</v>
@@ -6109,7 +6111,7 @@
         <v>581</v>
       </c>
       <c r="AF39" s="3" t="s">
-        <v>604</v>
+        <v>601</v>
       </c>
       <c r="AG39" s="3" t="s">
         <v>46</v>
@@ -6302,98 +6304,98 @@
         <v>46</v>
       </c>
     </row>
-    <row r="42" spans="1:33" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="5" t="s">
+    <row r="42" spans="1:33" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="4" t="s">
         <v>345</v>
       </c>
-      <c r="B42" s="5" t="s">
+      <c r="B42" s="4" t="s">
         <v>346</v>
       </c>
-      <c r="C42" s="5" t="s">
+      <c r="C42" s="4" t="s">
         <v>347</v>
       </c>
-      <c r="D42" s="5">
+      <c r="D42" s="4">
         <v>2016</v>
       </c>
-      <c r="E42" s="5">
-        <v>1</v>
-      </c>
-      <c r="F42" s="5">
-        <v>1</v>
-      </c>
-      <c r="G42" s="5" t="s">
+      <c r="E42" s="4">
+        <v>1</v>
+      </c>
+      <c r="F42" s="4">
+        <v>1</v>
+      </c>
+      <c r="G42" s="4" t="s">
         <v>240</v>
       </c>
-      <c r="H42" s="5" t="s">
+      <c r="H42" s="4" t="s">
         <v>241</v>
       </c>
-      <c r="I42" s="5">
+      <c r="I42" s="4">
         <v>153</v>
       </c>
-      <c r="J42" s="5">
+      <c r="J42" s="4">
         <v>13</v>
       </c>
-      <c r="K42" s="5" t="s">
+      <c r="K42" s="4" t="s">
         <v>348</v>
       </c>
-      <c r="L42" s="5" t="s">
+      <c r="L42" s="4" t="s">
         <v>349</v>
       </c>
-      <c r="M42" s="5" t="s">
+      <c r="M42" s="4" t="s">
         <v>350</v>
       </c>
-      <c r="O42" s="5" t="s">
+      <c r="O42" s="4" t="s">
         <v>245</v>
       </c>
-      <c r="Q42" s="5" t="s">
+      <c r="Q42" s="4" t="s">
         <v>351</v>
       </c>
-      <c r="R42" s="5" t="s">
+      <c r="R42" s="4" t="s">
         <v>127</v>
       </c>
-      <c r="S42" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="T42" s="5" t="s">
-        <v>581</v>
-      </c>
-      <c r="U42" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="V42" s="5" t="s">
-        <v>581</v>
-      </c>
-      <c r="W42" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="X42" s="5" t="s">
+      <c r="S42" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="T42" s="4" t="s">
+        <v>581</v>
+      </c>
+      <c r="U42" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="V42" s="4" t="s">
+        <v>581</v>
+      </c>
+      <c r="W42" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="X42" s="4" t="s">
         <v>584</v>
       </c>
-      <c r="Y42" s="5" t="s">
-        <v>639</v>
-      </c>
-      <c r="Z42" s="5" t="s">
-        <v>582</v>
-      </c>
-      <c r="AA42" s="5" t="s">
-        <v>581</v>
-      </c>
-      <c r="AB42" s="5" t="s">
-        <v>582</v>
-      </c>
-      <c r="AC42" s="5" t="s">
-        <v>581</v>
-      </c>
-      <c r="AD42" s="5" t="s">
-        <v>581</v>
-      </c>
-      <c r="AE42" s="5" t="s">
-        <v>582</v>
-      </c>
-      <c r="AF42" s="5" t="s">
-        <v>640</v>
-      </c>
-      <c r="AG42" s="5" t="s">
+      <c r="Y42" s="4" t="s">
+        <v>629</v>
+      </c>
+      <c r="Z42" s="4" t="s">
+        <v>582</v>
+      </c>
+      <c r="AA42" s="4" t="s">
+        <v>581</v>
+      </c>
+      <c r="AB42" s="4" t="s">
+        <v>582</v>
+      </c>
+      <c r="AC42" s="4" t="s">
+        <v>581</v>
+      </c>
+      <c r="AD42" s="4" t="s">
+        <v>581</v>
+      </c>
+      <c r="AE42" s="4" t="s">
+        <v>582</v>
+      </c>
+      <c r="AF42" s="4" t="s">
+        <v>630</v>
+      </c>
+      <c r="AG42" s="4" t="s">
         <v>46</v>
       </c>
     </row>
@@ -6483,101 +6485,101 @@
         <v>581</v>
       </c>
       <c r="AF43" s="3" t="s">
-        <v>641</v>
+        <v>631</v>
       </c>
       <c r="AG43" s="3" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="44" spans="1:33" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="5" t="s">
+    <row r="44" spans="1:33" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="4" t="s">
         <v>361</v>
       </c>
-      <c r="B44" s="5" t="s">
+      <c r="B44" s="4" t="s">
         <v>362</v>
       </c>
-      <c r="C44" s="5" t="s">
+      <c r="C44" s="4" t="s">
         <v>363</v>
       </c>
-      <c r="D44" s="5">
+      <c r="D44" s="4">
         <v>2018</v>
       </c>
-      <c r="E44" s="5">
-        <v>1</v>
-      </c>
-      <c r="F44" s="5">
-        <v>1</v>
-      </c>
-      <c r="G44" s="5" t="s">
+      <c r="E44" s="4">
+        <v>1</v>
+      </c>
+      <c r="F44" s="4">
+        <v>1</v>
+      </c>
+      <c r="G44" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="H44" s="5" t="s">
+      <c r="H44" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="I44" s="5">
+      <c r="I44" s="4">
         <v>142</v>
       </c>
-      <c r="K44" s="5" t="s">
+      <c r="K44" s="4" t="s">
         <v>364</v>
       </c>
-      <c r="L44" s="5" t="s">
+      <c r="L44" s="4" t="s">
         <v>365</v>
       </c>
-      <c r="M44" s="5" t="s">
+      <c r="M44" s="4" t="s">
         <v>366</v>
       </c>
-      <c r="O44" s="5" t="s">
+      <c r="O44" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="Q44" s="5" t="s">
+      <c r="Q44" s="4" t="s">
         <v>367</v>
       </c>
-      <c r="R44" s="5" t="s">
+      <c r="R44" s="4" t="s">
         <v>127</v>
       </c>
-      <c r="S44" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="T44" s="5" t="s">
-        <v>581</v>
-      </c>
-      <c r="U44" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="V44" s="5" t="s">
-        <v>581</v>
-      </c>
-      <c r="W44" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="X44" s="5" t="s">
+      <c r="S44" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="T44" s="4" t="s">
+        <v>581</v>
+      </c>
+      <c r="U44" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="V44" s="4" t="s">
+        <v>581</v>
+      </c>
+      <c r="W44" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="X44" s="4" t="s">
         <v>583</v>
       </c>
-      <c r="Y44" s="5" t="s">
-        <v>642</v>
-      </c>
-      <c r="Z44" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="AA44" s="5" t="s">
-        <v>643</v>
-      </c>
-      <c r="AB44" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="AC44" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="AD44" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="AE44" s="5" t="s">
-        <v>582</v>
-      </c>
-      <c r="AF44" s="5" t="s">
-        <v>644</v>
-      </c>
-      <c r="AG44" s="5" t="s">
+      <c r="Y44" s="4" t="s">
+        <v>632</v>
+      </c>
+      <c r="Z44" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="AA44" s="4" t="s">
+        <v>633</v>
+      </c>
+      <c r="AB44" s="4" t="s">
+        <v>582</v>
+      </c>
+      <c r="AC44" s="4" t="s">
+        <v>581</v>
+      </c>
+      <c r="AD44" s="4" t="s">
+        <v>581</v>
+      </c>
+      <c r="AE44" s="4" t="s">
+        <v>582</v>
+      </c>
+      <c r="AF44" s="4" t="s">
+        <v>634</v>
+      </c>
+      <c r="AG44" s="4" t="s">
         <v>46</v>
       </c>
     </row>
@@ -6738,13 +6740,13 @@
         <v>584</v>
       </c>
       <c r="Y46" s="1" t="s">
-        <v>645</v>
+        <v>685</v>
       </c>
       <c r="Z46" s="1" t="s">
         <v>44</v>
       </c>
       <c r="AA46" s="1" t="s">
-        <v>646</v>
+        <v>635</v>
       </c>
       <c r="AB46" s="1" t="s">
         <v>582</v>
@@ -6833,7 +6835,7 @@
         <v>583</v>
       </c>
       <c r="Y47" s="3" t="s">
-        <v>647</v>
+        <v>636</v>
       </c>
       <c r="Z47" s="4" t="s">
         <v>582</v>
@@ -6949,7 +6951,7 @@
         <v>581</v>
       </c>
       <c r="AF48" s="6" t="s">
-        <v>648</v>
+        <v>637</v>
       </c>
       <c r="AG48" s="6" t="s">
         <v>46</v>
@@ -7044,7 +7046,7 @@
         <v>581</v>
       </c>
       <c r="AF49" s="3" t="s">
-        <v>649</v>
+        <v>638</v>
       </c>
       <c r="AG49" s="3" t="s">
         <v>46</v>
@@ -7136,7 +7138,7 @@
         <v>581</v>
       </c>
       <c r="AF50" s="3" t="s">
-        <v>650</v>
+        <v>639</v>
       </c>
       <c r="AG50" s="3" t="s">
         <v>46</v>
@@ -7210,13 +7212,13 @@
         <v>584</v>
       </c>
       <c r="Y51" s="6" t="s">
-        <v>654</v>
+        <v>643</v>
       </c>
       <c r="Z51" s="6" t="s">
         <v>44</v>
       </c>
       <c r="AA51" s="6" t="s">
-        <v>653</v>
+        <v>642</v>
       </c>
       <c r="AB51" s="6" t="s">
         <v>44</v>
@@ -7225,13 +7227,13 @@
         <v>583</v>
       </c>
       <c r="AD51" s="6" t="s">
-        <v>652</v>
+        <v>641</v>
       </c>
       <c r="AE51" s="6" t="s">
         <v>582</v>
       </c>
       <c r="AF51" s="6" t="s">
-        <v>651</v>
+        <v>640</v>
       </c>
       <c r="AG51" s="6" t="s">
         <v>46</v>
@@ -7302,7 +7304,7 @@
         <v>44</v>
       </c>
       <c r="X52" s="7" t="s">
-        <v>636</v>
+        <v>627</v>
       </c>
       <c r="Y52" s="7" t="s">
         <v>581</v>
@@ -7326,7 +7328,7 @@
         <v>582</v>
       </c>
       <c r="AF52" s="7" t="s">
-        <v>655</v>
+        <v>644</v>
       </c>
       <c r="AG52" s="3" t="s">
         <v>46</v>
@@ -7489,13 +7491,13 @@
         <v>584</v>
       </c>
       <c r="Y54" s="6" t="s">
-        <v>656</v>
+        <v>645</v>
       </c>
       <c r="Z54" s="6" t="s">
         <v>44</v>
       </c>
       <c r="AA54" s="6" t="s">
-        <v>657</v>
+        <v>646</v>
       </c>
       <c r="AB54" s="7" t="s">
         <v>582</v>
@@ -7581,13 +7583,13 @@
         <v>583</v>
       </c>
       <c r="Y55" s="3" t="s">
-        <v>659</v>
+        <v>686</v>
       </c>
       <c r="Z55" s="7" t="s">
         <v>44</v>
       </c>
       <c r="AA55" s="3" t="s">
-        <v>658</v>
+        <v>687</v>
       </c>
       <c r="AB55" s="7" t="s">
         <v>582</v>
@@ -7676,7 +7678,7 @@
         <v>584</v>
       </c>
       <c r="Y56" s="3" t="s">
-        <v>660</v>
+        <v>688</v>
       </c>
       <c r="Z56" s="7" t="s">
         <v>582</v>
@@ -7688,7 +7690,7 @@
         <v>44</v>
       </c>
       <c r="AC56" s="7" t="s">
-        <v>636</v>
+        <v>627</v>
       </c>
       <c r="AD56" s="7" t="s">
         <v>581</v>
@@ -7697,7 +7699,7 @@
         <v>44</v>
       </c>
       <c r="AF56" s="7" t="s">
-        <v>661</v>
+        <v>647</v>
       </c>
       <c r="AG56" s="3" t="s">
         <v>46</v>
@@ -7768,19 +7770,19 @@
         <v>584</v>
       </c>
       <c r="Y57" s="3" t="s">
-        <v>663</v>
+        <v>649</v>
       </c>
       <c r="Z57" s="7" t="s">
-        <v>44</v>
+        <v>582</v>
       </c>
       <c r="AA57" s="7" t="s">
-        <v>662</v>
+        <v>648</v>
       </c>
       <c r="AB57" s="7" t="s">
         <v>582</v>
       </c>
-      <c r="AC57" s="7" t="s">
-        <v>665</v>
+      <c r="AC57" s="3" t="s">
+        <v>581</v>
       </c>
       <c r="AD57" s="7" t="s">
         <v>581</v>
@@ -7789,7 +7791,7 @@
         <v>582</v>
       </c>
       <c r="AF57" s="3" t="s">
-        <v>664</v>
+        <v>689</v>
       </c>
       <c r="AG57" s="3" t="s">
         <v>46</v>
@@ -7863,19 +7865,19 @@
         <v>583</v>
       </c>
       <c r="Y58" s="3" t="s">
-        <v>666</v>
+        <v>651</v>
       </c>
       <c r="Z58" s="7" t="s">
         <v>44</v>
       </c>
       <c r="AA58" s="3" t="s">
-        <v>667</v>
+        <v>652</v>
       </c>
       <c r="AB58" s="7" t="s">
         <v>582</v>
       </c>
-      <c r="AC58" s="7" t="s">
-        <v>665</v>
+      <c r="AC58" s="3" t="s">
+        <v>581</v>
       </c>
       <c r="AD58" s="7" t="s">
         <v>581</v>
@@ -7976,7 +7978,7 @@
         <v>581</v>
       </c>
       <c r="AF59" s="3" t="s">
-        <v>668</v>
+        <v>653</v>
       </c>
       <c r="AG59" s="3" t="s">
         <v>46</v>
@@ -8047,28 +8049,28 @@
         <v>584</v>
       </c>
       <c r="Y60" s="3" t="s">
-        <v>670</v>
+        <v>655</v>
       </c>
       <c r="Z60" s="3" t="s">
         <v>44</v>
       </c>
       <c r="AA60" s="3" t="s">
-        <v>671</v>
+        <v>656</v>
       </c>
       <c r="AB60" s="3" t="s">
         <v>44</v>
       </c>
       <c r="AC60" s="3" t="s">
-        <v>636</v>
+        <v>627</v>
       </c>
       <c r="AD60" s="3" t="s">
-        <v>669</v>
+        <v>654</v>
       </c>
       <c r="AE60" s="7" t="s">
         <v>582</v>
       </c>
       <c r="AF60" s="7" t="s">
-        <v>672</v>
+        <v>690</v>
       </c>
       <c r="AG60" s="3" t="s">
         <v>46</v>
@@ -8142,19 +8144,19 @@
         <v>583</v>
       </c>
       <c r="Y61" s="3" t="s">
-        <v>673</v>
+        <v>657</v>
       </c>
       <c r="Z61" s="3" t="s">
         <v>44</v>
       </c>
       <c r="AA61" s="3" t="s">
-        <v>674</v>
+        <v>658</v>
       </c>
       <c r="AB61" s="7" t="s">
         <v>582</v>
       </c>
-      <c r="AC61" s="7" t="s">
-        <v>665</v>
+      <c r="AC61" s="3" t="s">
+        <v>581</v>
       </c>
       <c r="AD61" s="7" t="s">
         <v>581</v>
@@ -8234,22 +8236,22 @@
         <v>584</v>
       </c>
       <c r="Y62" s="4" t="s">
-        <v>675</v>
+        <v>659</v>
       </c>
       <c r="Z62" s="4" t="s">
         <v>44</v>
       </c>
       <c r="AA62" s="4" t="s">
-        <v>676</v>
+        <v>660</v>
       </c>
       <c r="AB62" s="7" t="s">
         <v>44</v>
       </c>
       <c r="AC62" s="3" t="s">
-        <v>636</v>
+        <v>627</v>
       </c>
       <c r="AD62" s="7" t="s">
-        <v>665</v>
+        <v>650</v>
       </c>
       <c r="AE62" s="7" t="s">
         <v>44</v>
@@ -8326,19 +8328,19 @@
         <v>584</v>
       </c>
       <c r="Y63" s="4" t="s">
-        <v>678</v>
+        <v>662</v>
       </c>
       <c r="Z63" s="4" t="s">
         <v>44</v>
       </c>
       <c r="AA63" s="3" t="s">
-        <v>677</v>
+        <v>661</v>
       </c>
       <c r="AB63" s="7" t="s">
         <v>582</v>
       </c>
-      <c r="AC63" s="7" t="s">
-        <v>665</v>
+      <c r="AC63" s="3" t="s">
+        <v>581</v>
       </c>
       <c r="AD63" s="7" t="s">
         <v>581</v>
@@ -8421,7 +8423,7 @@
         <v>584</v>
       </c>
       <c r="Y64" s="4" t="s">
-        <v>679</v>
+        <v>663</v>
       </c>
       <c r="Z64" s="4" t="s">
         <v>582</v>
@@ -8442,7 +8444,7 @@
         <v>44</v>
       </c>
       <c r="AF64" s="4" t="s">
-        <v>680</v>
+        <v>664</v>
       </c>
       <c r="AG64" s="4" t="s">
         <v>46</v>
@@ -8605,13 +8607,13 @@
         <v>584</v>
       </c>
       <c r="Y66" s="3" t="s">
-        <v>682</v>
+        <v>666</v>
       </c>
       <c r="Z66" s="3" t="s">
         <v>44</v>
       </c>
       <c r="AA66" s="3" t="s">
-        <v>683</v>
+        <v>667</v>
       </c>
       <c r="AB66" s="4" t="s">
         <v>582</v>
@@ -8626,7 +8628,7 @@
         <v>582</v>
       </c>
       <c r="AF66" s="3" t="s">
-        <v>681</v>
+        <v>665</v>
       </c>
       <c r="AG66" s="3" t="s">
         <v>46</v>
@@ -8700,7 +8702,7 @@
         <v>584</v>
       </c>
       <c r="Y67" s="3" t="s">
-        <v>684</v>
+        <v>668</v>
       </c>
       <c r="Z67" s="4" t="s">
         <v>582</v>
@@ -8813,7 +8815,7 @@
         <v>581</v>
       </c>
       <c r="AF68" s="3" t="s">
-        <v>685</v>
+        <v>669</v>
       </c>
       <c r="AG68" s="3" t="s">
         <v>46</v>
@@ -8979,13 +8981,13 @@
         <v>584</v>
       </c>
       <c r="Y70" s="3" t="s">
-        <v>687</v>
+        <v>671</v>
       </c>
       <c r="Z70" s="3" t="s">
         <v>44</v>
       </c>
       <c r="AA70" s="3" t="s">
-        <v>686</v>
+        <v>670</v>
       </c>
       <c r="AB70" s="4" t="s">
         <v>582</v>
@@ -9068,10 +9070,10 @@
         <v>44</v>
       </c>
       <c r="X71" s="8" t="s">
-        <v>586</v>
+        <v>584</v>
       </c>
       <c r="Y71" s="5" t="s">
-        <v>688</v>
+        <v>672</v>
       </c>
       <c r="Z71" s="5" t="s">
         <v>582</v>
@@ -9092,7 +9094,7 @@
         <v>44</v>
       </c>
       <c r="AF71" s="5" t="s">
-        <v>689</v>
+        <v>691</v>
       </c>
       <c r="AG71" s="5" t="s">
         <v>46</v>
@@ -9353,7 +9355,7 @@
         <v>583</v>
       </c>
       <c r="Y74" s="3" t="s">
-        <v>690</v>
+        <v>673</v>
       </c>
       <c r="Z74" s="4" t="s">
         <v>582</v>
@@ -9374,7 +9376,7 @@
         <v>582</v>
       </c>
       <c r="AF74" s="3" t="s">
-        <v>691</v>
+        <v>692</v>
       </c>
       <c r="AG74" s="3" t="s">
         <v>46</v>

</xml_diff>